<commit_message>
validated import and added total size
</commit_message>
<xml_diff>
--- a/EnergyCert/WebContent/client/sites.xlsx
+++ b/EnergyCert/WebContent/client/sites.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8250"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Region</t>
   </si>
@@ -30,10 +30,13 @@
     <t>Street</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>Postal</t>
+  </si>
+  <si>
+    <t>Total Size</t>
+  </si>
+  <si>
+    <t>City/ State</t>
   </si>
 </sst>
 </file>
@@ -372,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,9 +397,12 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>